<commit_message>
cleaning up, sim equations
</commit_message>
<xml_diff>
--- a/results/probability_data_only_theta.xlsx
+++ b/results/probability_data_only_theta.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ChrisWiseLocal\GitHub\ZEIT3191-ML-Quantum-Computing\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4809E20A-25E8-4F86-80EA-B484E75F55A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{017AB0A1-0127-44B0-82CB-AC1332755F61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1545" yWindow="2325" windowWidth="21600" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="probability_data_only_theta" sheetId="1" r:id="rId1"/>
@@ -639,8 +639,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>